<commit_message>
Updated Budd Inlet figures
</commit_message>
<xml_diff>
--- a/BuddInlet/Data/DinoXToxinData.xlsx
+++ b/BuddInlet/Data/DinoXToxinData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexis.fischer/Documents/MATLAB/bloom-baby-bloom/NOAA/BuddInlet/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexis.fischer/Documents/MATLAB/bloom-baby-bloom/BuddInlet/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A1B24C-6F6A-EF47-8313-B3FBC02BF9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88819B58-1156-A443-9D03-0FCC9ABD36B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="500" windowWidth="37820" windowHeight="22540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="183">
   <si>
     <t>SIEVE TOX DATA:  Surfside, TX</t>
   </si>
@@ -728,9 +728,6 @@
   </si>
   <si>
     <t>Lost sample</t>
-  </si>
-  <si>
-    <t>no volume on tube</t>
   </si>
   <si>
     <t>2022*</t>
@@ -7028,8 +7025,8 @@
   <dimension ref="A1:Z1032"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R8" sqref="R8"/>
+      <pane ySplit="8" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7051,19 +7048,19 @@
     </row>
     <row r="2" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="211" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H2" s="212"/>
     </row>
     <row r="3" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="211" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H3" s="212"/>
     </row>
     <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="211" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H4" s="212"/>
     </row>
@@ -7133,16 +7130,16 @@
         <v>14</v>
       </c>
       <c r="I8" s="221" t="s">
+        <v>170</v>
+      </c>
+      <c r="J8" s="217" t="s">
         <v>171</v>
       </c>
-      <c r="J8" s="217" t="s">
+      <c r="K8" s="217" t="s">
         <v>172</v>
       </c>
-      <c r="K8" s="217" t="s">
+      <c r="L8" s="217" t="s">
         <v>173</v>
-      </c>
-      <c r="L8" s="217" t="s">
-        <v>174</v>
       </c>
       <c r="M8" s="222" t="s">
         <v>19</v>
@@ -7151,31 +7148,31 @@
         <v>20</v>
       </c>
       <c r="O8" s="223" t="s">
+        <v>174</v>
+      </c>
+      <c r="P8" s="223" t="s">
         <v>175</v>
       </c>
-      <c r="P8" s="223" t="s">
+      <c r="Q8" s="223" t="s">
         <v>176</v>
       </c>
-      <c r="Q8" s="223" t="s">
+      <c r="R8" s="223" t="s">
         <v>177</v>
-      </c>
-      <c r="R8" s="223" t="s">
-        <v>178</v>
       </c>
       <c r="S8" s="223" t="s">
         <v>25</v>
       </c>
       <c r="T8" s="224" t="s">
+        <v>178</v>
+      </c>
+      <c r="U8" s="225" t="s">
         <v>179</v>
       </c>
-      <c r="U8" s="225" t="s">
+      <c r="V8" s="225" t="s">
         <v>180</v>
       </c>
-      <c r="V8" s="225" t="s">
+      <c r="W8" s="225" t="s">
         <v>181</v>
-      </c>
-      <c r="W8" s="225" t="s">
-        <v>182</v>
       </c>
       <c r="X8" s="226" t="s">
         <v>30</v>
@@ -10286,15 +10283,15 @@
         <v>1</v>
       </c>
       <c r="E50" s="260"/>
-      <c r="F50" s="244" t="s">
-        <v>68</v>
+      <c r="F50" s="244">
+        <v>4</v>
       </c>
       <c r="G50" s="244">
         <v>667</v>
       </c>
-      <c r="H50" s="245" t="e">
+      <c r="H50" s="245">
         <f t="shared" si="52"/>
-        <v>#VALUE!</v>
+        <v>2668</v>
       </c>
       <c r="I50" s="261">
         <v>0</v>
@@ -10334,25 +10331,25 @@
         <f t="shared" si="79"/>
         <v>79.043704268292686</v>
       </c>
-      <c r="T50" s="248" t="e">
+      <c r="T50" s="248">
         <f t="shared" ref="T50:X50" si="80">O50/$H50</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="U50" s="249" t="e">
+        <v>0</v>
+      </c>
+      <c r="U50" s="249">
         <f t="shared" si="80"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="V50" s="249" t="e">
+        <v>3.4191863861760372E-3</v>
+      </c>
+      <c r="V50" s="249">
         <f t="shared" si="80"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="W50" s="249" t="e">
+        <v>0</v>
+      </c>
+      <c r="W50" s="249">
         <f t="shared" si="80"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="X50" s="250" t="e">
+        <v>0</v>
+      </c>
+      <c r="X50" s="250">
         <f t="shared" si="80"/>
-        <v>#VALUE!</v>
+        <v>2.9626575812703407E-2</v>
       </c>
       <c r="Z50" s="286">
         <v>20157.469000000001</v>
@@ -10370,15 +10367,15 @@
         <v>1.5</v>
       </c>
       <c r="E51" s="260"/>
-      <c r="F51" s="244" t="s">
-        <v>68</v>
+      <c r="F51" s="244">
+        <v>4</v>
       </c>
       <c r="G51" s="244">
         <v>2250</v>
       </c>
-      <c r="H51" s="245" t="e">
+      <c r="H51" s="245">
         <f t="shared" si="52"/>
-        <v>#VALUE!</v>
+        <v>9000</v>
       </c>
       <c r="I51" s="261">
         <v>0</v>
@@ -10418,25 +10415,25 @@
         <f t="shared" si="81"/>
         <v>282.06789634146338</v>
       </c>
-      <c r="T51" s="248" t="e">
+      <c r="T51" s="248">
         <f t="shared" ref="T51:X51" si="82">O51/$H51</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="U51" s="249" t="e">
+        <v>0</v>
+      </c>
+      <c r="U51" s="249">
         <f t="shared" si="82"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="V51" s="249" t="e">
+        <v>5.5977663161807644E-3</v>
+      </c>
+      <c r="V51" s="249">
         <f t="shared" si="82"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="W51" s="249" t="e">
+        <v>0</v>
+      </c>
+      <c r="W51" s="249">
         <f t="shared" si="82"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="X51" s="250" t="e">
+        <v>0</v>
+      </c>
+      <c r="X51" s="250">
         <f t="shared" si="82"/>
-        <v>#VALUE!</v>
+        <v>3.1340877371273709E-2</v>
       </c>
       <c r="Z51" s="286">
         <v>130623.04700000001</v>
@@ -11284,7 +11281,7 @@
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="228" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B62" s="214" t="s">
         <v>65</v>
@@ -12085,7 +12082,7 @@
         <v>2.553685022492786E-5</v>
       </c>
       <c r="U71" s="249">
-        <f t="shared" ref="T71:X71" si="122">P71/$H71</f>
+        <f t="shared" ref="U71:X71" si="122">P71/$H71</f>
         <v>1.8580074212897579E-3</v>
       </c>
       <c r="V71" s="249">
@@ -12167,7 +12164,7 @@
         <v>0</v>
       </c>
       <c r="U72" s="249">
-        <f t="shared" ref="T72:X72" si="124">P72/$H72</f>
+        <f t="shared" ref="U72:X72" si="124">P72/$H72</f>
         <v>7.5994790292798729E-3</v>
       </c>
       <c r="V72" s="249">
@@ -14921,7 +14918,7 @@
     </row>
     <row r="119" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="211" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F119" s="386"/>
       <c r="H119" s="212"/>
@@ -14939,7 +14936,7 @@
     </row>
     <row r="120" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="211" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F120" s="386"/>
       <c r="H120" s="212"/>
@@ -14957,7 +14954,7 @@
     </row>
     <row r="121" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="211" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F121" s="386"/>
       <c r="H121" s="212"/>
@@ -18704,7 +18701,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
@@ -18720,7 +18717,7 @@
     </row>
     <row r="2" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
@@ -18736,7 +18733,7 @@
     </row>
     <row r="3" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="42"/>
       <c r="C3" s="42"/>
@@ -18752,7 +18749,7 @@
     </row>
     <row r="4" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
@@ -18850,16 +18847,16 @@
         <v>14</v>
       </c>
       <c r="H8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="J8" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="K8" s="10" t="s">
         <v>78</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>79</v>
       </c>
       <c r="L8" s="11" t="s">
         <v>19</v>
@@ -18868,31 +18865,31 @@
         <v>20</v>
       </c>
       <c r="N8" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="O8" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="O8" s="12" t="s">
+      <c r="P8" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="Q8" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="Q8" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="R8" s="141" t="s">
         <v>25</v>
       </c>
       <c r="S8" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="T8" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="T8" s="14" t="s">
+      <c r="U8" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="U8" s="14" t="s">
+      <c r="V8" s="14" t="s">
         <v>86</v>
-      </c>
-      <c r="V8" s="14" t="s">
-        <v>87</v>
       </c>
       <c r="W8" s="15" t="s">
         <v>30</v>
@@ -18906,10 +18903,10 @@
         <v>2018</v>
       </c>
       <c r="B9" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="142" t="s">
         <v>88</v>
-      </c>
-      <c r="C9" s="142" t="s">
-        <v>89</v>
       </c>
       <c r="D9" s="96"/>
       <c r="E9" s="97"/>
@@ -18977,10 +18974,10 @@
     <row r="10" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="99"/>
       <c r="B10" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="143" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="100"/>
       <c r="E10" s="101"/>
@@ -19048,10 +19045,10 @@
     <row r="11" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="99"/>
       <c r="B11" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="143" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="100"/>
       <c r="E11" s="101"/>
@@ -19119,10 +19116,10 @@
     <row r="12" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="99"/>
       <c r="B12" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" s="143" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" s="100"/>
       <c r="E12" s="101"/>
@@ -19190,10 +19187,10 @@
     <row r="13" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="99"/>
       <c r="B13" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="143" t="s">
         <v>91</v>
-      </c>
-      <c r="C13" s="143" t="s">
-        <v>92</v>
       </c>
       <c r="D13" s="100"/>
       <c r="E13" s="101"/>
@@ -19261,10 +19258,10 @@
     <row r="14" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="99"/>
       <c r="B14" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="143" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="100"/>
       <c r="E14" s="101"/>
@@ -19332,10 +19329,10 @@
     <row r="15" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="99"/>
       <c r="B15" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" s="143" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" s="100"/>
       <c r="E15" s="101"/>
@@ -19403,10 +19400,10 @@
     <row r="16" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="99"/>
       <c r="B16" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" s="143" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D16" s="100"/>
       <c r="E16" s="101"/>
@@ -19474,10 +19471,10 @@
     <row r="17" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="99"/>
       <c r="B17" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="143" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" s="100"/>
       <c r="E17" s="101"/>
@@ -19545,10 +19542,10 @@
     <row r="18" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="99"/>
       <c r="B18" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" s="143" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D18" s="100"/>
       <c r="E18" s="101"/>
@@ -19616,10 +19613,10 @@
     <row r="19" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="99"/>
       <c r="B19" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" s="143" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D19" s="100"/>
       <c r="E19" s="101"/>
@@ -19687,10 +19684,10 @@
     <row r="20" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="99"/>
       <c r="B20" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C20" s="143" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" s="100"/>
       <c r="E20" s="101"/>
@@ -19758,10 +19755,10 @@
     <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="99"/>
       <c r="B21" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" s="143" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21" s="100"/>
       <c r="E21" s="101"/>
@@ -19829,10 +19826,10 @@
     <row r="22" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="99"/>
       <c r="B22" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C22" s="143" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="100"/>
       <c r="E22" s="101"/>
@@ -19900,10 +19897,10 @@
     <row r="23" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="99"/>
       <c r="B23" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="143" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D23" s="100"/>
       <c r="E23" s="101"/>
@@ -19971,10 +19968,10 @@
     <row r="24" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="41"/>
       <c r="B24" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" s="143" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D24" s="59"/>
       <c r="E24" s="60"/>
@@ -20042,10 +20039,10 @@
     <row r="25" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="99"/>
       <c r="B25" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" s="143" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D25" s="59"/>
       <c r="E25" s="60"/>
@@ -20113,10 +20110,10 @@
     <row r="26" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="99"/>
       <c r="B26" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C26" s="143" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D26" s="59"/>
       <c r="E26" s="60"/>
@@ -20184,10 +20181,10 @@
     <row r="27" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="99"/>
       <c r="B27" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27" s="143" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D27" s="59"/>
       <c r="E27" s="60"/>
@@ -20255,10 +20252,10 @@
     <row r="28" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="99"/>
       <c r="B28" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" s="143" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D28" s="59"/>
       <c r="E28" s="60"/>
@@ -20326,10 +20323,10 @@
     <row r="29" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="99"/>
       <c r="B29" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C29" s="143" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D29" s="59"/>
       <c r="E29" s="60"/>
@@ -20397,10 +20394,10 @@
     <row r="30" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="99"/>
       <c r="B30" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" s="143" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D30" s="59"/>
       <c r="E30" s="60"/>
@@ -20468,10 +20465,10 @@
     <row r="31" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="99"/>
       <c r="B31" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C31" s="143" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D31" s="59"/>
       <c r="E31" s="60"/>
@@ -20539,10 +20536,10 @@
     <row r="32" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="99"/>
       <c r="B32" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C32" s="143" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D32" s="59"/>
       <c r="E32" s="60"/>
@@ -20610,10 +20607,10 @@
     <row r="33" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="41"/>
       <c r="B33" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="143" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D33" s="59"/>
       <c r="E33" s="60"/>
@@ -20681,10 +20678,10 @@
     <row r="34" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="99"/>
       <c r="B34" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C34" s="143" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D34" s="59"/>
       <c r="E34" s="60"/>
@@ -20752,10 +20749,10 @@
     <row r="35" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="127"/>
       <c r="B35" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C35" s="143" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D35" s="59"/>
       <c r="E35" s="144"/>
@@ -20823,10 +20820,10 @@
     <row r="36" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="127"/>
       <c r="B36" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" s="143" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D36" s="59"/>
       <c r="E36" s="144"/>
@@ -20894,10 +20891,10 @@
     <row r="37" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="127"/>
       <c r="B37" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C37" s="143" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D37" s="59"/>
       <c r="E37" s="144"/>
@@ -20965,10 +20962,10 @@
     <row r="38" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="127"/>
       <c r="B38" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C38" s="143" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D38" s="59"/>
       <c r="E38" s="129"/>
@@ -21036,10 +21033,10 @@
     <row r="39" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="127"/>
       <c r="B39" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39" s="143" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D39" s="59"/>
       <c r="E39" s="129"/>
@@ -21107,10 +21104,10 @@
     <row r="40" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="127"/>
       <c r="B40" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C40" s="143" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D40" s="59"/>
       <c r="E40" s="129"/>
@@ -21178,10 +21175,10 @@
     <row r="41" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="127"/>
       <c r="B41" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41" s="143" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D41" s="59"/>
       <c r="E41" s="144"/>
@@ -21249,10 +21246,10 @@
     <row r="42" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="127"/>
       <c r="B42" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C42" s="143" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D42" s="59"/>
       <c r="E42" s="144"/>
@@ -21320,10 +21317,10 @@
     <row r="43" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="127"/>
       <c r="B43" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C43" s="143" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D43" s="59"/>
       <c r="E43" s="144"/>
@@ -21391,10 +21388,10 @@
     <row r="44" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="127"/>
       <c r="B44" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C44" s="143" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D44" s="59"/>
       <c r="E44" s="144"/>
@@ -21462,10 +21459,10 @@
     <row r="45" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="127"/>
       <c r="B45" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C45" s="143" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D45" s="59"/>
       <c r="E45" s="144"/>
@@ -21535,7 +21532,7 @@
         <v>2019</v>
       </c>
       <c r="B46" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C46" s="145">
         <v>43556</v>
@@ -21606,7 +21603,7 @@
     <row r="47" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="127"/>
       <c r="B47" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C47" s="149">
         <v>43556</v>
@@ -21677,7 +21674,7 @@
     <row r="48" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="127"/>
       <c r="B48" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C48" s="149">
         <v>43563</v>
@@ -21748,7 +21745,7 @@
     <row r="49" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="127"/>
       <c r="B49" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C49" s="149">
         <v>43571</v>
@@ -21819,7 +21816,7 @@
     <row r="50" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="127"/>
       <c r="B50" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C50" s="149">
         <v>43571</v>
@@ -21890,7 +21887,7 @@
     <row r="51" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="127"/>
       <c r="B51" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C51" s="149">
         <v>43577</v>
@@ -21961,7 +21958,7 @@
     <row r="52" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="127"/>
       <c r="B52" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C52" s="149">
         <v>43584</v>
@@ -22032,7 +22029,7 @@
     <row r="53" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="127"/>
       <c r="B53" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C53" s="149">
         <v>43584</v>
@@ -22103,7 +22100,7 @@
     <row r="54" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="127"/>
       <c r="B54" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C54" s="149">
         <v>43585</v>
@@ -22174,7 +22171,7 @@
     <row r="55" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="127"/>
       <c r="B55" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C55" s="149">
         <v>43591</v>
@@ -22245,7 +22242,7 @@
     <row r="56" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="127"/>
       <c r="B56" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C56" s="149">
         <v>43592</v>
@@ -22316,7 +22313,7 @@
     <row r="57" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="127"/>
       <c r="B57" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C57" s="149">
         <v>43592</v>
@@ -22387,7 +22384,7 @@
     <row r="58" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="127"/>
       <c r="B58" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C58" s="149">
         <v>43598</v>
@@ -22458,7 +22455,7 @@
     <row r="59" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="127"/>
       <c r="B59" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C59" s="149">
         <v>43598</v>
@@ -22529,7 +22526,7 @@
     <row r="60" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="127"/>
       <c r="B60" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C60" s="149">
         <v>43599</v>
@@ -22600,7 +22597,7 @@
     <row r="61" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="127"/>
       <c r="B61" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C61" s="149">
         <v>43605</v>
@@ -22671,7 +22668,7 @@
     <row r="62" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="127"/>
       <c r="B62" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C62" s="149">
         <v>43609</v>
@@ -22742,7 +22739,7 @@
     <row r="63" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="127"/>
       <c r="B63" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C63" s="149">
         <v>43609</v>
@@ -22813,7 +22810,7 @@
     <row r="64" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="127"/>
       <c r="B64" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C64" s="149">
         <v>43613</v>
@@ -22884,7 +22881,7 @@
     <row r="65" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="127"/>
       <c r="B65" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C65" s="149">
         <v>43613</v>
@@ -22955,7 +22952,7 @@
     <row r="66" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="127"/>
       <c r="B66" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C66" s="149">
         <v>43613</v>
@@ -23026,7 +23023,7 @@
     <row r="67" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="127"/>
       <c r="B67" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C67" s="149">
         <v>43619</v>
@@ -23097,7 +23094,7 @@
     <row r="68" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="127"/>
       <c r="B68" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C68" s="149">
         <v>43619</v>
@@ -23168,7 +23165,7 @@
     <row r="69" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="127"/>
       <c r="B69" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C69" s="149">
         <v>43619</v>
@@ -23239,7 +23236,7 @@
     <row r="70" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="127"/>
       <c r="B70" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C70" s="149">
         <v>43626</v>
@@ -23310,7 +23307,7 @@
     <row r="71" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="127"/>
       <c r="B71" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C71" s="149">
         <v>43626</v>
@@ -23381,7 +23378,7 @@
     <row r="72" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="127"/>
       <c r="B72" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C72" s="149">
         <v>43626</v>
@@ -23452,7 +23449,7 @@
     <row r="73" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="127"/>
       <c r="B73" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C73" s="149">
         <v>43633</v>
@@ -23523,7 +23520,7 @@
     <row r="74" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="127"/>
       <c r="B74" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C74" s="149">
         <v>43633</v>
@@ -23594,7 +23591,7 @@
     <row r="75" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="127"/>
       <c r="B75" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C75" s="149">
         <v>43633</v>
@@ -23665,7 +23662,7 @@
     <row r="76" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="127"/>
       <c r="B76" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C76" s="149">
         <v>43640</v>
@@ -23736,7 +23733,7 @@
     <row r="77" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="127"/>
       <c r="B77" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C77" s="149">
         <v>43640</v>
@@ -23807,7 +23804,7 @@
     <row r="78" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="127"/>
       <c r="B78" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C78" s="149">
         <v>43640</v>
@@ -23878,7 +23875,7 @@
     <row r="79" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="127"/>
       <c r="B79" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C79" s="149">
         <v>43647</v>
@@ -23949,7 +23946,7 @@
     <row r="80" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="127"/>
       <c r="B80" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C80" s="149">
         <v>43647</v>
@@ -24020,7 +24017,7 @@
     <row r="81" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="127"/>
       <c r="B81" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C81" s="149">
         <v>43647</v>
@@ -24091,7 +24088,7 @@
     <row r="82" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="127"/>
       <c r="B82" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C82" s="149">
         <v>43654</v>
@@ -24162,7 +24159,7 @@
     <row r="83" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="127"/>
       <c r="B83" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C83" s="149">
         <v>43654</v>
@@ -24233,7 +24230,7 @@
     <row r="84" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="127"/>
       <c r="B84" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C84" s="149">
         <v>43654</v>
@@ -24304,7 +24301,7 @@
     <row r="85" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="127"/>
       <c r="B85" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C85" s="149">
         <v>43661</v>
@@ -24375,7 +24372,7 @@
     <row r="86" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="127"/>
       <c r="B86" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C86" s="149">
         <v>43661</v>
@@ -24446,7 +24443,7 @@
     <row r="87" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="127"/>
       <c r="B87" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C87" s="149">
         <v>43661</v>
@@ -24517,7 +24514,7 @@
     <row r="88" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="127"/>
       <c r="B88" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C88" s="149">
         <v>43668</v>
@@ -24588,7 +24585,7 @@
     <row r="89" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="127"/>
       <c r="B89" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C89" s="149">
         <v>43668</v>
@@ -24659,7 +24656,7 @@
     <row r="90" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="127"/>
       <c r="B90" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C90" s="149">
         <v>43668</v>
@@ -24730,7 +24727,7 @@
     <row r="91" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="127"/>
       <c r="B91" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C91" s="149">
         <v>43675</v>
@@ -24801,7 +24798,7 @@
     <row r="92" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="116"/>
       <c r="B92" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C92" s="152">
         <v>43675</v>
@@ -24871,10 +24868,10 @@
     </row>
     <row r="93" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B93" s="103" t="s">
         <v>106</v>
-      </c>
-      <c r="B93" s="103" t="s">
-        <v>107</v>
       </c>
       <c r="C93" s="119">
         <v>43950</v>
@@ -24948,7 +24945,7 @@
     <row r="94" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="127"/>
       <c r="B94" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C94" s="123">
         <v>43950</v>
@@ -25022,7 +25019,7 @@
     <row r="95" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="127"/>
       <c r="B95" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C95" s="123">
         <v>43950</v>
@@ -25096,7 +25093,7 @@
     <row r="96" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="122"/>
       <c r="B96" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C96" s="123">
         <v>43950</v>
@@ -25170,7 +25167,7 @@
     <row r="97" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="122"/>
       <c r="B97" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C97" s="123">
         <v>43950</v>
@@ -25244,7 +25241,7 @@
     <row r="98" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="122"/>
       <c r="B98" s="109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C98" s="123">
         <v>43957</v>
@@ -25318,7 +25315,7 @@
     <row r="99" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="122"/>
       <c r="B99" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C99" s="123">
         <v>43957</v>
@@ -25392,7 +25389,7 @@
     <row r="100" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="122"/>
       <c r="B100" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C100" s="123">
         <v>43957</v>
@@ -25466,7 +25463,7 @@
     <row r="101" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="127"/>
       <c r="B101" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C101" s="123">
         <v>43957</v>
@@ -25540,7 +25537,7 @@
     <row r="102" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="127"/>
       <c r="B102" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C102" s="123">
         <v>43957</v>
@@ -25614,7 +25611,7 @@
     <row r="103" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="127"/>
       <c r="B103" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C103" s="123">
         <v>43962</v>
@@ -25688,7 +25685,7 @@
     <row r="104" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="127"/>
       <c r="B104" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C104" s="123">
         <v>43962</v>
@@ -25764,7 +25761,7 @@
     <row r="105" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="127"/>
       <c r="B105" s="109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C105" s="123">
         <v>43964</v>
@@ -25838,7 +25835,7 @@
     <row r="106" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="127"/>
       <c r="B106" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C106" s="123">
         <v>43964</v>
@@ -25912,7 +25909,7 @@
     <row r="107" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="122"/>
       <c r="B107" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C107" s="123">
         <v>43964</v>
@@ -25988,7 +25985,7 @@
     <row r="108" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="122"/>
       <c r="B108" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C108" s="123">
         <v>43969</v>
@@ -26064,7 +26061,7 @@
     <row r="109" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="122"/>
       <c r="B109" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C109" s="123">
         <v>43969</v>
@@ -26140,7 +26137,7 @@
     <row r="110" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="122"/>
       <c r="B110" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C110" s="123">
         <v>43969</v>
@@ -26214,7 +26211,7 @@
     <row r="111" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="122"/>
       <c r="B111" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C111" s="123">
         <v>43969</v>
@@ -26290,7 +26287,7 @@
     <row r="112" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="122"/>
       <c r="B112" s="109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C112" s="123">
         <v>43971</v>
@@ -26364,7 +26361,7 @@
     <row r="113" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="122"/>
       <c r="B113" s="109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C113" s="123">
         <v>43978</v>
@@ -26440,7 +26437,7 @@
     <row r="114" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="122"/>
       <c r="B114" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C114" s="123">
         <v>43978</v>
@@ -26516,7 +26513,7 @@
     <row r="115" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="122"/>
       <c r="B115" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C115" s="123">
         <v>43978</v>
@@ -26592,7 +26589,7 @@
     <row r="116" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="122"/>
       <c r="B116" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C116" s="123">
         <v>43978</v>
@@ -26668,7 +26665,7 @@
     <row r="117" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="122"/>
       <c r="B117" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C117" s="123">
         <v>43978</v>
@@ -26744,7 +26741,7 @@
     <row r="118" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="122"/>
       <c r="B118" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C118" s="123">
         <v>43983</v>
@@ -26820,7 +26817,7 @@
     <row r="119" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="122"/>
       <c r="B119" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C119" s="123">
         <v>43983</v>
@@ -26896,7 +26893,7 @@
     <row r="120" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="122"/>
       <c r="B120" s="109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C120" s="123">
         <v>43985</v>
@@ -26972,7 +26969,7 @@
     <row r="121" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="122"/>
       <c r="B121" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C121" s="123">
         <v>43985</v>
@@ -27046,7 +27043,7 @@
     <row r="122" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="122"/>
       <c r="B122" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C122" s="123">
         <v>43985</v>
@@ -27120,7 +27117,7 @@
     <row r="123" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="122"/>
       <c r="B123" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C123" s="123">
         <v>43990</v>
@@ -27196,7 +27193,7 @@
     <row r="124" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="122"/>
       <c r="B124" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C124" s="123">
         <v>43990</v>
@@ -27272,7 +27269,7 @@
     <row r="125" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="122"/>
       <c r="B125" s="109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C125" s="123">
         <v>43992</v>
@@ -27348,7 +27345,7 @@
     <row r="126" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="122"/>
       <c r="B126" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C126" s="123">
         <v>43992</v>
@@ -27424,7 +27421,7 @@
     <row r="127" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="122"/>
       <c r="B127" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C127" s="123">
         <v>43992</v>
@@ -27500,7 +27497,7 @@
     <row r="128" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="122"/>
       <c r="B128" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C128" s="123">
         <v>43997</v>
@@ -27576,7 +27573,7 @@
     <row r="129" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="122"/>
       <c r="B129" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C129" s="123">
         <v>43997</v>
@@ -27652,7 +27649,7 @@
     <row r="130" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="122"/>
       <c r="B130" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C130" s="123">
         <v>43997</v>
@@ -27726,7 +27723,7 @@
     <row r="131" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="122"/>
       <c r="B131" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C131" s="123">
         <v>43997</v>
@@ -27802,7 +27799,7 @@
     <row r="132" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="122"/>
       <c r="B132" s="109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C132" s="123">
         <v>43999</v>
@@ -27878,7 +27875,7 @@
     <row r="133" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="122"/>
       <c r="B133" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C133" s="123">
         <v>44004</v>
@@ -27952,7 +27949,7 @@
     <row r="134" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="122"/>
       <c r="B134" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C134" s="123">
         <v>44004</v>
@@ -28028,7 +28025,7 @@
     <row r="135" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="122"/>
       <c r="B135" s="109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C135" s="123">
         <v>44006</v>
@@ -28102,7 +28099,7 @@
     <row r="136" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="122"/>
       <c r="B136" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C136" s="123">
         <v>44006</v>
@@ -28178,7 +28175,7 @@
     <row r="137" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="122"/>
       <c r="B137" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C137" s="123">
         <v>44006</v>
@@ -28254,7 +28251,7 @@
     <row r="138" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="122"/>
       <c r="B138" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C138" s="123">
         <v>44011</v>
@@ -28330,7 +28327,7 @@
     <row r="139" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="122"/>
       <c r="B139" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C139" s="123">
         <v>44011</v>
@@ -28406,7 +28403,7 @@
     <row r="140" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="122"/>
       <c r="B140" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C140" s="123">
         <v>44012</v>
@@ -28482,7 +28479,7 @@
     <row r="141" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="122"/>
       <c r="B141" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C141" s="123">
         <v>44013</v>
@@ -28558,7 +28555,7 @@
     <row r="142" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="122"/>
       <c r="B142" s="109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C142" s="123">
         <v>44018</v>
@@ -28634,7 +28631,7 @@
     <row r="143" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="122"/>
       <c r="B143" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C143" s="123">
         <v>44018</v>
@@ -28710,7 +28707,7 @@
     <row r="144" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="122"/>
       <c r="B144" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C144" s="123">
         <v>44018</v>
@@ -28786,7 +28783,7 @@
     <row r="145" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="122"/>
       <c r="B145" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C145" s="123">
         <v>44020</v>
@@ -28862,7 +28859,7 @@
     <row r="146" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="122"/>
       <c r="B146" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C146" s="123">
         <v>44020</v>
@@ -28938,7 +28935,7 @@
     <row r="147" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="122"/>
       <c r="B147" s="109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C147" s="123">
         <v>44025</v>
@@ -29014,7 +29011,7 @@
     <row r="148" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="122"/>
       <c r="B148" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C148" s="123">
         <v>44025</v>
@@ -29090,7 +29087,7 @@
     <row r="149" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="122"/>
       <c r="B149" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C149" s="123">
         <v>44025</v>
@@ -29164,7 +29161,7 @@
     <row r="150" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="122"/>
       <c r="B150" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C150" s="123">
         <v>44026</v>
@@ -29238,7 +29235,7 @@
     <row r="151" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="122"/>
       <c r="B151" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C151" s="123">
         <v>44026</v>
@@ -29314,7 +29311,7 @@
     <row r="152" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="122"/>
       <c r="B152" s="109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C152" s="123">
         <v>44032</v>
@@ -29390,7 +29387,7 @@
     <row r="153" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="122"/>
       <c r="B153" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C153" s="123">
         <v>44032</v>
@@ -29464,7 +29461,7 @@
     <row r="154" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="122"/>
       <c r="B154" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C154" s="123">
         <v>44032</v>
@@ -29538,7 +29535,7 @@
     <row r="155" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="122"/>
       <c r="B155" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C155" s="123">
         <v>44032</v>
@@ -29612,7 +29609,7 @@
     <row r="156" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="122"/>
       <c r="B156" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C156" s="123">
         <v>44032</v>
@@ -29686,7 +29683,7 @@
     <row r="157" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="122"/>
       <c r="B157" s="109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C157" s="123">
         <v>44039</v>
@@ -29760,7 +29757,7 @@
     <row r="158" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="122"/>
       <c r="B158" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C158" s="123">
         <v>44039</v>
@@ -29834,7 +29831,7 @@
     <row r="159" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="122"/>
       <c r="B159" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C159" s="123">
         <v>44039</v>
@@ -29910,7 +29907,7 @@
     <row r="160" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="122"/>
       <c r="B160" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C160" s="123">
         <v>44041</v>
@@ -29984,7 +29981,7 @@
     <row r="161" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="122"/>
       <c r="B161" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C161" s="123">
         <v>44041</v>
@@ -30058,7 +30055,7 @@
     <row r="162" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="122"/>
       <c r="B162" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C162" s="123">
         <v>44048</v>
@@ -30134,7 +30131,7 @@
     <row r="163" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="122"/>
       <c r="B163" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C163" s="123">
         <v>44048</v>
@@ -30208,7 +30205,7 @@
     <row r="164" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="122"/>
       <c r="B164" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C164" s="123">
         <v>44055</v>
@@ -30282,7 +30279,7 @@
     <row r="165" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="130"/>
       <c r="B165" s="117" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C165" s="131">
         <v>44055</v>
@@ -30358,7 +30355,7 @@
         <v>64</v>
       </c>
       <c r="B166" s="103" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C166" s="119">
         <v>44291</v>
@@ -30432,7 +30429,7 @@
     <row r="167" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="122"/>
       <c r="B167" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C167" s="123">
         <v>44291</v>
@@ -30506,7 +30503,7 @@
     <row r="168" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="122"/>
       <c r="B168" s="109" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C168" s="123">
         <v>44298</v>
@@ -30580,7 +30577,7 @@
     <row r="169" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="122"/>
       <c r="B169" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C169" s="123">
         <v>44299</v>
@@ -30654,7 +30651,7 @@
     <row r="170" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="122"/>
       <c r="B170" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C170" s="123">
         <v>44305</v>
@@ -30728,7 +30725,7 @@
     <row r="171" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="122"/>
       <c r="B171" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C171" s="123">
         <v>44305</v>
@@ -30802,7 +30799,7 @@
     <row r="172" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="122"/>
       <c r="B172" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C172" s="123">
         <v>44306</v>
@@ -30876,7 +30873,7 @@
     <row r="173" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="122"/>
       <c r="B173" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C173" s="123">
         <v>44312</v>
@@ -30950,7 +30947,7 @@
     <row r="174" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="122"/>
       <c r="B174" s="109" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C174" s="123">
         <v>44312</v>
@@ -31024,7 +31021,7 @@
     <row r="175" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="122"/>
       <c r="B175" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C175" s="123">
         <v>44319</v>
@@ -31098,7 +31095,7 @@
     <row r="176" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="122"/>
       <c r="B176" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C176" s="123">
         <v>44320</v>
@@ -31172,7 +31169,7 @@
     <row r="177" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="122"/>
       <c r="B177" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C177" s="123">
         <v>44323</v>
@@ -31246,7 +31243,7 @@
     <row r="178" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="122"/>
       <c r="B178" s="109" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C178" s="123">
         <v>44326</v>
@@ -31320,7 +31317,7 @@
     <row r="179" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="122"/>
       <c r="B179" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C179" s="123">
         <v>44333</v>
@@ -31393,10 +31390,10 @@
     </row>
     <row r="180" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="176" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B180" s="177" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C180" s="178">
         <v>44333</v>
@@ -31428,7 +31425,7 @@
     <row r="181" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="122"/>
       <c r="B181" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C181" s="123">
         <v>44333</v>
@@ -31502,7 +31499,7 @@
     <row r="182" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="122"/>
       <c r="B182" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C182" s="123">
         <v>44333</v>
@@ -31576,7 +31573,7 @@
     <row r="183" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="122"/>
       <c r="B183" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C183" s="123">
         <v>44340</v>
@@ -31650,7 +31647,7 @@
     <row r="184" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="122"/>
       <c r="B184" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C184" s="123">
         <v>44340</v>
@@ -31724,7 +31721,7 @@
     <row r="185" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="122"/>
       <c r="B185" s="109" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C185" s="123">
         <v>44340</v>
@@ -31798,7 +31795,7 @@
     <row r="186" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="122"/>
       <c r="B186" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C186" s="123">
         <v>44340</v>
@@ -31872,7 +31869,7 @@
     <row r="187" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="122"/>
       <c r="B187" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C187" s="123">
         <v>44340</v>
@@ -31946,7 +31943,7 @@
     <row r="188" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="122"/>
       <c r="B188" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C188" s="123">
         <v>44348</v>
@@ -32020,7 +32017,7 @@
     <row r="189" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="122"/>
       <c r="B189" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C189" s="123">
         <v>44348</v>
@@ -32094,7 +32091,7 @@
     <row r="190" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="122"/>
       <c r="B190" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C190" s="123">
         <v>44348</v>
@@ -32168,7 +32165,7 @@
     <row r="191" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="122"/>
       <c r="B191" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C191" s="123">
         <v>44348</v>
@@ -32242,7 +32239,7 @@
     <row r="192" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="122"/>
       <c r="B192" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C192" s="123">
         <v>44348</v>
@@ -32316,7 +32313,7 @@
     <row r="193" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="122"/>
       <c r="B193" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C193" s="123">
         <v>44348</v>
@@ -32390,7 +32387,7 @@
     <row r="194" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="122"/>
       <c r="B194" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C194" s="123">
         <v>44354</v>
@@ -32464,7 +32461,7 @@
     <row r="195" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="122"/>
       <c r="B195" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C195" s="123">
         <v>44354</v>
@@ -32538,7 +32535,7 @@
     <row r="196" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="122"/>
       <c r="B196" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C196" s="123">
         <v>44354</v>
@@ -32614,7 +32611,7 @@
     <row r="197" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="122"/>
       <c r="B197" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C197" s="123">
         <v>44354</v>
@@ -32689,10 +32686,10 @@
     </row>
     <row r="198" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="176" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B198" s="177" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C198" s="178">
         <v>44359</v>
@@ -32724,7 +32721,7 @@
     <row r="199" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="122"/>
       <c r="B199" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C199" s="123">
         <v>44361</v>
@@ -32800,7 +32797,7 @@
     <row r="200" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="122"/>
       <c r="B200" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C200" s="123">
         <v>44361</v>
@@ -32874,7 +32871,7 @@
     <row r="201" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="122"/>
       <c r="B201" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C201" s="123">
         <v>44361</v>
@@ -32950,7 +32947,7 @@
     <row r="202" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="122"/>
       <c r="B202" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C202" s="123">
         <v>44361</v>
@@ -33026,7 +33023,7 @@
     <row r="203" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="122"/>
       <c r="B203" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C203" s="123">
         <v>44368</v>
@@ -33100,7 +33097,7 @@
     <row r="204" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="122"/>
       <c r="B204" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C204" s="123">
         <v>44368</v>
@@ -33174,7 +33171,7 @@
     <row r="205" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="122"/>
       <c r="B205" s="109" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C205" s="123">
         <v>44368</v>
@@ -33248,7 +33245,7 @@
     <row r="206" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="122"/>
       <c r="B206" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C206" s="123">
         <v>44368</v>
@@ -33324,7 +33321,7 @@
     <row r="207" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="122"/>
       <c r="B207" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C207" s="123">
         <v>44375</v>
@@ -33398,7 +33395,7 @@
     <row r="208" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="122"/>
       <c r="B208" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C208" s="123">
         <v>44375</v>
@@ -33472,7 +33469,7 @@
     <row r="209" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="122"/>
       <c r="B209" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C209" s="123">
         <v>44376</v>
@@ -33546,7 +33543,7 @@
     <row r="210" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="122"/>
       <c r="B210" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C210" s="123">
         <v>44376</v>
@@ -33622,7 +33619,7 @@
     <row r="211" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="122"/>
       <c r="B211" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C211" s="123">
         <v>44382</v>
@@ -33696,7 +33693,7 @@
     <row r="212" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="122"/>
       <c r="B212" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C212" s="123">
         <v>44382</v>
@@ -33770,7 +33767,7 @@
     <row r="213" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="122"/>
       <c r="B213" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C213" s="123">
         <v>44382</v>
@@ -33844,7 +33841,7 @@
     <row r="214" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="122"/>
       <c r="B214" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C214" s="123">
         <v>44382</v>
@@ -33920,7 +33917,7 @@
     <row r="215" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="122"/>
       <c r="B215" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C215" s="123">
         <v>44389</v>
@@ -33996,7 +33993,7 @@
     <row r="216" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="122"/>
       <c r="B216" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C216" s="123">
         <v>44389</v>
@@ -34072,7 +34069,7 @@
     <row r="217" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="122"/>
       <c r="B217" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C217" s="123">
         <v>44390</v>
@@ -34146,7 +34143,7 @@
     <row r="218" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="122"/>
       <c r="B218" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C218" s="123">
         <v>44390</v>
@@ -34220,7 +34217,7 @@
     <row r="219" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="122"/>
       <c r="B219" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C219" s="123">
         <v>44396</v>
@@ -34296,7 +34293,7 @@
     <row r="220" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="122"/>
       <c r="B220" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C220" s="123">
         <v>44396</v>
@@ -34372,7 +34369,7 @@
     <row r="221" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="122"/>
       <c r="B221" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C221" s="123">
         <v>44397</v>
@@ -34446,7 +34443,7 @@
     <row r="222" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="122"/>
       <c r="B222" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C222" s="123">
         <v>44397</v>
@@ -34520,7 +34517,7 @@
     <row r="223" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="122"/>
       <c r="B223" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C223" s="123">
         <v>44403</v>
@@ -34594,7 +34591,7 @@
     <row r="224" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="122"/>
       <c r="B224" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C224" s="123">
         <v>44403</v>
@@ -34668,7 +34665,7 @@
     <row r="225" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="122"/>
       <c r="B225" s="109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C225" s="123">
         <v>44404</v>
@@ -34742,7 +34739,7 @@
     <row r="226" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="122"/>
       <c r="B226" s="109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C226" s="123">
         <v>44404</v>
@@ -34816,7 +34813,7 @@
     <row r="227" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="122"/>
       <c r="B227" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C227" s="123">
         <v>44410</v>
@@ -34890,7 +34887,7 @@
     <row r="228" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="122"/>
       <c r="B228" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C228" s="123">
         <v>44410</v>
@@ -34964,7 +34961,7 @@
     <row r="229" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="122"/>
       <c r="B229" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C229" s="123">
         <v>44417</v>
@@ -35038,7 +35035,7 @@
     <row r="230" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="122"/>
       <c r="B230" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C230" s="123">
         <v>44417</v>
@@ -35112,7 +35109,7 @@
     <row r="231" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="122"/>
       <c r="B231" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C231" s="123">
         <v>44424</v>
@@ -35186,7 +35183,7 @@
     <row r="232" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="122"/>
       <c r="B232" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C232" s="123">
         <v>44424</v>
@@ -35259,10 +35256,10 @@
     </row>
     <row r="233" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="176" t="s">
+        <v>114</v>
+      </c>
+      <c r="B233" s="177" t="s">
         <v>115</v>
-      </c>
-      <c r="B233" s="177" t="s">
-        <v>116</v>
       </c>
       <c r="C233" s="178">
         <v>44368</v>
@@ -35337,10 +35334,10 @@
     </row>
     <row r="234" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="168" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B234" s="103" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C234" s="186">
         <v>44720</v>
@@ -35416,7 +35413,7 @@
     <row r="235" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="122"/>
       <c r="B235" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C235" s="187">
         <v>44728</v>
@@ -35492,7 +35489,7 @@
     <row r="236" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="122"/>
       <c r="B236" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C236" s="187">
         <v>44734</v>
@@ -35568,7 +35565,7 @@
     <row r="237" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="122"/>
       <c r="B237" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C237" s="187">
         <v>44741</v>
@@ -35642,7 +35639,7 @@
     <row r="238" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="122"/>
       <c r="B238" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C238" s="187">
         <v>44748</v>
@@ -35718,7 +35715,7 @@
     <row r="239" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="122"/>
       <c r="B239" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C239" s="187">
         <v>44755</v>
@@ -35794,7 +35791,7 @@
     <row r="240" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="122"/>
       <c r="B240" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C240" s="187">
         <v>44762</v>
@@ -35870,7 +35867,7 @@
     <row r="241" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="122"/>
       <c r="B241" s="109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C241" s="187">
         <v>44769</v>
@@ -35946,7 +35943,7 @@
     <row r="242" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="122"/>
       <c r="B242" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C242" s="187">
         <v>44706</v>
@@ -36020,7 +36017,7 @@
     <row r="243" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="122"/>
       <c r="B243" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C243" s="187">
         <v>44720</v>
@@ -36094,7 +36091,7 @@
     <row r="244" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="122"/>
       <c r="B244" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C244" s="187">
         <v>44728</v>
@@ -36170,7 +36167,7 @@
     <row r="245" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="122"/>
       <c r="B245" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C245" s="187">
         <v>44734</v>
@@ -36244,7 +36241,7 @@
     <row r="246" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="122"/>
       <c r="B246" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C246" s="187">
         <v>44741</v>
@@ -36318,7 +36315,7 @@
     <row r="247" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="122"/>
       <c r="B247" s="109" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C247" s="187">
         <v>44748</v>
@@ -36394,7 +36391,7 @@
     <row r="248" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="122"/>
       <c r="B248" s="109" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C248" s="187">
         <v>44725</v>
@@ -36470,7 +36467,7 @@
     <row r="249" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="122"/>
       <c r="B249" s="109" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C249" s="187">
         <v>44706</v>
@@ -36544,7 +36541,7 @@
     <row r="250" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="122"/>
       <c r="B250" s="109" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C250" s="187">
         <v>44708</v>
@@ -36620,7 +36617,7 @@
     <row r="251" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="122"/>
       <c r="B251" s="109" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C251" s="187">
         <v>44741</v>
@@ -36694,7 +36691,7 @@
     <row r="252" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="122"/>
       <c r="B252" s="109" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C252" s="187">
         <v>44748</v>
@@ -36768,7 +36765,7 @@
     <row r="253" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="122"/>
       <c r="B253" s="109" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C253" s="187">
         <v>44706</v>
@@ -36842,7 +36839,7 @@
     <row r="254" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="122"/>
       <c r="B254" s="109" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C254" s="187">
         <v>44708</v>
@@ -36918,7 +36915,7 @@
     <row r="255" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="122"/>
       <c r="B255" s="94" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C255" s="187">
         <v>44725</v>
@@ -36994,7 +36991,7 @@
     <row r="256" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="122"/>
       <c r="B256" s="94" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C256" s="187">
         <v>44706</v>
@@ -37068,7 +37065,7 @@
     <row r="257" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="122"/>
       <c r="B257" s="94" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C257" s="187">
         <v>44703</v>
@@ -37142,7 +37139,7 @@
     <row r="258" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="122"/>
       <c r="B258" s="94" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C258" s="187">
         <v>44725</v>
@@ -37216,7 +37213,7 @@
     <row r="259" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="130"/>
       <c r="B259" s="188" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C259" s="189">
         <v>44725</v>
@@ -37324,21 +37321,21 @@
     </row>
     <row r="266" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B266" s="109"/>
       <c r="C266" s="109"/>
     </row>
     <row r="267" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B267" s="109"/>
       <c r="C267" s="109"/>
     </row>
     <row r="268" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B268" s="109"/>
       <c r="C268" s="109"/>
@@ -40304,7 +40301,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
@@ -40321,7 +40318,7 @@
     </row>
     <row r="2" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
@@ -40338,7 +40335,7 @@
     </row>
     <row r="3" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" s="42"/>
       <c r="C3" s="42"/>
@@ -40355,7 +40352,7 @@
     </row>
     <row r="4" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
@@ -40456,16 +40453,16 @@
         <v>14</v>
       </c>
       <c r="H8" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="I8" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="J8" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="K8" s="10" t="s">
         <v>133</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>134</v>
       </c>
       <c r="L8" s="11" t="s">
         <v>19</v>
@@ -40474,31 +40471,31 @@
         <v>20</v>
       </c>
       <c r="N8" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="O8" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="O8" s="12" t="s">
+      <c r="P8" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="Q8" s="12" t="s">
         <v>137</v>
-      </c>
-      <c r="Q8" s="12" t="s">
-        <v>138</v>
       </c>
       <c r="R8" s="141" t="s">
         <v>25</v>
       </c>
       <c r="S8" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="T8" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="T8" s="14" t="s">
+      <c r="U8" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="U8" s="14" t="s">
+      <c r="V8" s="14" t="s">
         <v>141</v>
-      </c>
-      <c r="V8" s="14" t="s">
-        <v>142</v>
       </c>
       <c r="W8" s="15" t="s">
         <v>30</v>
@@ -40512,10 +40509,10 @@
         <v>2018</v>
       </c>
       <c r="B9" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>143</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>144</v>
       </c>
       <c r="D9" s="191">
         <v>9</v>
@@ -40592,13 +40589,13 @@
     </row>
     <row r="10" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="195" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>145</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>146</v>
       </c>
       <c r="D10" s="191">
         <v>17</v>
@@ -40676,10 +40673,10 @@
     <row r="11" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="22"/>
       <c r="B11" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D11" s="191">
         <v>17</v>
@@ -40756,13 +40753,13 @@
     </row>
     <row r="12" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="195" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C12" s="65" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D12" s="191">
         <v>9</v>
@@ -40840,10 +40837,10 @@
     <row r="13" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="22"/>
       <c r="B13" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D13" s="191">
         <v>5</v>
@@ -40920,13 +40917,13 @@
     </row>
     <row r="14" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="195" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D14" s="191">
         <v>2</v>
@@ -41004,10 +41001,10 @@
     <row r="15" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="22"/>
       <c r="B15" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D15" s="191">
         <v>9</v>
@@ -41084,13 +41081,13 @@
     </row>
     <row r="16" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="195" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D16" s="191">
         <v>16</v>
@@ -41168,10 +41165,10 @@
     <row r="17" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="22"/>
       <c r="B17" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D17" s="191">
         <v>12</v>
@@ -41248,13 +41245,13 @@
     </row>
     <row r="18" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="195" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D18" s="191">
         <v>25</v>
@@ -41332,10 +41329,10 @@
     <row r="19" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="22"/>
       <c r="B19" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D19" s="191">
         <v>11</v>
@@ -41412,13 +41409,13 @@
     </row>
     <row r="20" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="195" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D20" s="191">
         <v>20</v>
@@ -41496,10 +41493,10 @@
     <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="22"/>
       <c r="B21" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D21" s="191">
         <v>0</v>
@@ -41576,13 +41573,13 @@
     </row>
     <row r="22" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="195" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D22" s="191">
         <v>1</v>
@@ -41660,10 +41657,10 @@
     <row r="23" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="22"/>
       <c r="B23" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D23" s="191">
         <v>12</v>
@@ -41740,13 +41737,13 @@
     </row>
     <row r="24" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="195" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D24" s="191">
         <v>95</v>
@@ -41824,10 +41821,10 @@
     <row r="25" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="22"/>
       <c r="B25" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D25" s="191">
         <v>0</v>
@@ -41904,13 +41901,13 @@
     </row>
     <row r="26" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="195" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D26" s="191">
         <v>0</v>
@@ -41988,10 +41985,10 @@
     <row r="27" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="22"/>
       <c r="B27" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D27" s="191">
         <v>1</v>
@@ -42068,7 +42065,7 @@
         <v>2019</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C28" s="196">
         <v>43538</v>
@@ -42139,7 +42136,7 @@
     <row r="29" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="197"/>
       <c r="B29" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C29" s="198">
         <v>43543</v>
@@ -42210,7 +42207,7 @@
     <row r="30" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="197"/>
       <c r="B30" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C30" s="198">
         <v>43549</v>
@@ -42281,7 +42278,7 @@
     <row r="31" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="197"/>
       <c r="B31" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C31" s="198">
         <v>43556</v>
@@ -42352,7 +42349,7 @@
     <row r="32" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="197"/>
       <c r="B32" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C32" s="198">
         <v>43563</v>
@@ -42423,7 +42420,7 @@
     <row r="33" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="197"/>
       <c r="B33" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C33" s="198">
         <v>43570</v>
@@ -42494,7 +42491,7 @@
     <row r="34" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="197"/>
       <c r="B34" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C34" s="198">
         <v>43577</v>
@@ -42565,7 +42562,7 @@
     <row r="35" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="197"/>
       <c r="B35" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C35" s="198">
         <v>43588</v>
@@ -42636,7 +42633,7 @@
     <row r="36" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="197"/>
       <c r="B36" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C36" s="198">
         <v>43594</v>
@@ -42707,7 +42704,7 @@
     <row r="37" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="197"/>
       <c r="B37" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C37" s="198">
         <v>43599</v>
@@ -42778,7 +42775,7 @@
     <row r="38" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="197"/>
       <c r="B38" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C38" s="198">
         <v>43606</v>
@@ -42849,7 +42846,7 @@
     <row r="39" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="197"/>
       <c r="B39" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C39" s="198">
         <v>43613</v>
@@ -42920,7 +42917,7 @@
     <row r="40" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="197"/>
       <c r="B40" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C40" s="198">
         <v>43619</v>
@@ -42991,7 +42988,7 @@
     <row r="41" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="197"/>
       <c r="B41" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C41" s="198">
         <v>43626</v>
@@ -43064,7 +43061,7 @@
         <v>2020</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C42" s="196">
         <v>43846</v>
@@ -43145,7 +43142,7 @@
     <row r="43" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="197"/>
       <c r="B43" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C43" s="198">
         <v>43854</v>
@@ -43226,7 +43223,7 @@
     <row r="44" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="197"/>
       <c r="B44" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C44" s="198">
         <v>43861</v>
@@ -43307,7 +43304,7 @@
     <row r="45" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="197"/>
       <c r="B45" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C45" s="198">
         <v>43868</v>
@@ -43388,7 +43385,7 @@
     <row r="46" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="197"/>
       <c r="B46" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C46" s="65">
         <v>43875</v>
@@ -43469,7 +43466,7 @@
     <row r="47" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="197"/>
       <c r="B47" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C47" s="65">
         <v>43882</v>
@@ -43550,7 +43547,7 @@
     <row r="48" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="197"/>
       <c r="B48" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C48" s="65">
         <v>43889</v>
@@ -43631,7 +43628,7 @@
     <row r="49" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="197"/>
       <c r="B49" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C49" s="65">
         <v>43897</v>
@@ -43712,7 +43709,7 @@
     <row r="50" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="197"/>
       <c r="B50" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C50" s="65">
         <v>43903</v>
@@ -43793,7 +43790,7 @@
     <row r="51" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="197"/>
       <c r="B51" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C51" s="65">
         <v>43911</v>
@@ -43874,7 +43871,7 @@
     <row r="52" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="197"/>
       <c r="B52" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C52" s="65">
         <v>43917</v>
@@ -43955,7 +43952,7 @@
     <row r="53" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="197"/>
       <c r="B53" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C53" s="65">
         <v>43924</v>
@@ -44036,7 +44033,7 @@
     <row r="54" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="197"/>
       <c r="B54" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C54" s="65">
         <v>43938</v>
@@ -44117,7 +44114,7 @@
     <row r="55" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="197"/>
       <c r="B55" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C55" s="65">
         <v>43952</v>
@@ -44198,7 +44195,7 @@
     <row r="56" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="197"/>
       <c r="B56" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C56" s="65">
         <v>43966</v>
@@ -44279,7 +44276,7 @@
     <row r="57" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="197"/>
       <c r="B57" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C57" s="65">
         <v>43980</v>
@@ -44360,7 +44357,7 @@
     <row r="58" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="197"/>
       <c r="B58" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C58" s="65">
         <v>43994</v>
@@ -44441,7 +44438,7 @@
     <row r="59" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="197"/>
       <c r="B59" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C59" s="65">
         <v>44007</v>
@@ -44522,7 +44519,7 @@
     <row r="60" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="197"/>
       <c r="B60" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C60" s="65">
         <v>44022</v>
@@ -44603,7 +44600,7 @@
     <row r="61" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="197"/>
       <c r="B61" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C61" s="65">
         <v>44036</v>
@@ -44684,13 +44681,13 @@
     <row r="62" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="197"/>
       <c r="B62" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C62" s="65">
         <v>44050</v>
       </c>
       <c r="D62" s="100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E62" s="124">
         <v>8</v>
@@ -44759,13 +44756,13 @@
     <row r="63" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="197"/>
       <c r="B63" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C63" s="65">
         <v>44067</v>
       </c>
       <c r="D63" s="100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E63" s="124">
         <v>8</v>
@@ -44773,7 +44770,7 @@
       <c r="F63" s="60"/>
       <c r="G63" s="61"/>
       <c r="H63" s="201" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I63" s="112"/>
       <c r="J63" s="112"/>
@@ -44794,13 +44791,13 @@
     <row r="64" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="197"/>
       <c r="B64" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C64" s="65">
         <v>44078</v>
       </c>
       <c r="D64" s="100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E64" s="124">
         <v>8</v>
@@ -44869,13 +44866,13 @@
     <row r="65" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="197"/>
       <c r="B65" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C65" s="65">
         <v>44097</v>
       </c>
       <c r="D65" s="100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E65" s="124">
         <v>8</v>
@@ -44944,13 +44941,13 @@
     <row r="66" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="197"/>
       <c r="B66" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C66" s="65">
         <v>44106</v>
       </c>
       <c r="D66" s="100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E66" s="124">
         <v>8</v>
@@ -45019,13 +45016,13 @@
     <row r="67" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="197"/>
       <c r="B67" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C67" s="65">
         <v>44119</v>
       </c>
       <c r="D67" s="100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E67" s="124">
         <v>8</v>
@@ -45094,13 +45091,13 @@
     <row r="68" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="197"/>
       <c r="B68" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C68" s="65">
         <v>44134</v>
       </c>
       <c r="D68" s="100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E68" s="124">
         <v>8</v>
@@ -45169,13 +45166,13 @@
     <row r="69" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="197"/>
       <c r="B69" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C69" s="65">
         <v>44153</v>
       </c>
       <c r="D69" s="100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E69" s="124"/>
       <c r="F69" s="60"/>
@@ -45242,13 +45239,13 @@
     <row r="70" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="197"/>
       <c r="B70" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C70" s="65">
         <v>44169</v>
       </c>
       <c r="D70" s="100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E70" s="124">
         <v>8</v>
@@ -45317,13 +45314,13 @@
     <row r="71" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="197"/>
       <c r="B71" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C71" s="65">
         <v>44183</v>
       </c>
       <c r="D71" s="100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E71" s="124">
         <v>8</v>
@@ -45394,13 +45391,13 @@
         <v>2021</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C72" s="66">
         <v>44204</v>
       </c>
       <c r="D72" s="96" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E72" s="146"/>
       <c r="F72" s="54"/>
@@ -45467,13 +45464,13 @@
     <row r="73" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="122"/>
       <c r="B73" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C73" s="65">
         <v>44223</v>
       </c>
       <c r="D73" s="100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E73" s="129"/>
       <c r="F73" s="60"/>
@@ -45540,13 +45537,13 @@
     <row r="74" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="122"/>
       <c r="B74" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C74" s="65">
         <v>44249</v>
       </c>
       <c r="D74" s="100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E74" s="129"/>
       <c r="F74" s="60"/>
@@ -45613,7 +45610,7 @@
     <row r="75" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="122"/>
       <c r="B75" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C75" s="65">
         <v>44264</v>
@@ -45686,7 +45683,7 @@
     <row r="76" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="122"/>
       <c r="B76" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C76" s="65">
         <v>44278</v>
@@ -45759,7 +45756,7 @@
     <row r="77" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="122"/>
       <c r="B77" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C77" s="65">
         <v>44292</v>
@@ -45832,7 +45829,7 @@
     <row r="78" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="122"/>
       <c r="B78" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C78" s="65">
         <v>44306</v>
@@ -45905,7 +45902,7 @@
     <row r="79" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="122"/>
       <c r="B79" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C79" s="65">
         <v>44320</v>
@@ -45978,7 +45975,7 @@
     <row r="80" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="122"/>
       <c r="B80" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C80" s="65">
         <v>44343</v>
@@ -46049,7 +46046,7 @@
     <row r="81" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="122"/>
       <c r="B81" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C81" s="65">
         <v>44365</v>
@@ -46120,7 +46117,7 @@
     <row r="82" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="122"/>
       <c r="B82" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C82" s="65">
         <v>44378</v>
@@ -46191,7 +46188,7 @@
     <row r="83" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="122"/>
       <c r="B83" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C83" s="65">
         <v>44393</v>
@@ -46262,7 +46259,7 @@
     <row r="84" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="122"/>
       <c r="B84" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C84" s="65">
         <v>44407</v>
@@ -46333,7 +46330,7 @@
     <row r="85" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="122"/>
       <c r="B85" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C85" s="65">
         <v>44432</v>
@@ -46404,7 +46401,7 @@
     <row r="86" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="122"/>
       <c r="B86" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C86" s="65">
         <v>44448</v>
@@ -46475,7 +46472,7 @@
     <row r="87" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="122"/>
       <c r="B87" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C87" s="65">
         <v>44462</v>
@@ -46546,7 +46543,7 @@
     <row r="88" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="122"/>
       <c r="B88" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C88" s="65">
         <v>44477</v>
@@ -46617,7 +46614,7 @@
     <row r="89" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="122"/>
       <c r="B89" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C89" s="65">
         <v>44491</v>
@@ -46688,7 +46685,7 @@
     <row r="90" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="122"/>
       <c r="B90" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C90" s="65">
         <v>44505</v>
@@ -46759,7 +46756,7 @@
     <row r="91" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="122"/>
       <c r="B91" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C91" s="65">
         <v>44519</v>
@@ -46830,7 +46827,7 @@
     <row r="92" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="122"/>
       <c r="B92" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C92" s="65">
         <v>44533</v>
@@ -46901,7 +46898,7 @@
     <row r="93" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="130"/>
       <c r="B93" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C93" s="69">
         <v>44546</v>
@@ -46971,10 +46968,10 @@
     </row>
     <row r="94" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C94" s="145">
         <v>44568</v>
@@ -47048,7 +47045,7 @@
     <row r="95" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="41"/>
       <c r="B95" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C95" s="149">
         <v>44580</v>
@@ -47122,7 +47119,7 @@
     <row r="96" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="41"/>
       <c r="B96" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C96" s="149">
         <v>44596</v>
@@ -47196,7 +47193,7 @@
     <row r="97" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="41"/>
       <c r="B97" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C97" s="149">
         <v>44608</v>
@@ -47270,7 +47267,7 @@
     <row r="98" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="41"/>
       <c r="B98" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C98" s="149">
         <v>44622</v>
@@ -47344,7 +47341,7 @@
     <row r="99" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="41"/>
       <c r="B99" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C99" s="149">
         <v>44629</v>
@@ -47418,7 +47415,7 @@
     <row r="100" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="41"/>
       <c r="B100" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C100" s="149">
         <v>44637</v>
@@ -47492,7 +47489,7 @@
     <row r="101" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="41"/>
       <c r="B101" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C101" s="149">
         <v>44643</v>
@@ -47566,7 +47563,7 @@
     <row r="102" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="41"/>
       <c r="B102" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C102" s="149">
         <v>44650</v>
@@ -47640,7 +47637,7 @@
     <row r="103" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="41"/>
       <c r="B103" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C103" s="149">
         <v>44657</v>
@@ -47714,7 +47711,7 @@
     <row r="104" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="41"/>
       <c r="B104" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C104" s="149">
         <v>44666</v>
@@ -47788,7 +47785,7 @@
     <row r="105" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="41"/>
       <c r="B105" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C105" s="149">
         <v>44673</v>
@@ -47862,7 +47859,7 @@
     <row r="106" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="41"/>
       <c r="B106" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C106" s="149">
         <v>44679</v>
@@ -47936,7 +47933,7 @@
     <row r="107" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="41"/>
       <c r="B107" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C107" s="149">
         <v>44685</v>
@@ -48010,7 +48007,7 @@
     <row r="108" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="41"/>
       <c r="B108" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C108" s="149">
         <v>44693</v>
@@ -48084,7 +48081,7 @@
     <row r="109" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="41"/>
       <c r="B109" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C109" s="149">
         <v>44699</v>
@@ -48158,7 +48155,7 @@
     <row r="110" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="41"/>
       <c r="B110" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C110" s="149">
         <v>44707</v>
@@ -48232,7 +48229,7 @@
     <row r="111" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="67"/>
       <c r="B111" s="68" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C111" s="152">
         <v>44713</v>
@@ -48399,7 +48396,7 @@
     </row>
     <row r="116" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B116" s="42"/>
       <c r="C116" s="42"/>
@@ -48423,7 +48420,7 @@
     </row>
     <row r="117" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B117" s="42"/>
       <c r="C117" s="42"/>
@@ -48447,7 +48444,7 @@
     </row>
     <row r="118" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B118" s="42"/>
       <c r="C118" s="42"/>

</xml_diff>